<commit_message>
HW2 resubmit figures pdf
</commit_message>
<xml_diff>
--- a/Working/HW2_BoxModel_manual/starter_code/HW_02_Heter_boxlayer.xlsx
+++ b/Working/HW2_BoxModel_manual/starter_code/HW_02_Heter_boxlayer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\Groundwater Modeling\Local Repository\homework-JakeSmith1993\Working\HW2_BoxModel_manual\starter_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B86BF39-766F-44CF-A69B-AEB1E12EF4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36095B16-571A-4F27-93F3-73D53A6C00BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{E797DA87-9764-CF40-B10D-4CBD1F0C2290}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E797DA87-9764-CF40-B10D-4CBD1F0C2290}"/>
   </bookViews>
   <sheets>
     <sheet name="bcf_1_edited" sheetId="3" r:id="rId1"/>
@@ -14423,7 +14423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E986F2-53D6-1C4D-B056-8DFA12526A7B}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -25656,7 +25656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B181C23-F43C-6848-921C-DFC38BE5DD7E}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -28330,8 +28330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B7FEA8-679C-6245-B574-9BBD7BB6F993}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>